<commit_message>
feat: Initial project setup and core functionalities
</commit_message>
<xml_diff>
--- a/planilha_temas.xlsx
+++ b/planilha_temas.xlsx
@@ -1,96 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Pyton\ttk-app\app-tiktok\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F2B0BF-6B27-4B8F-8DFA-7AAFAA9B60AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t>Tema</t>
-  </si>
-  <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Relevância</t>
-  </si>
-  <si>
-    <t>Roteiro</t>
-  </si>
-  <si>
-    <t>Video Pronto</t>
-  </si>
-  <si>
-    <t>Video Postado</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>O Objeto Interestelar 3I/ATLAS</t>
-  </si>
-  <si>
-    <t>O misterioso objeto 3I/ATLAS é o ponto central da maior parte do conteúdo, gerando intensas discussões sobre sua natureza – se é um cometa, um asteroide, um visitante de outra estrela ou até uma nave alienígena – e seu trajeto próximo ao Sol ou à Terra, com menções a datas específicas para revelações.</t>
-  </si>
-  <si>
-    <t>alta</t>
-  </si>
-  <si>
-    <t>Especulações sobre Vida Extraterrestre e Mistérios Cósmicos</t>
-  </si>
-  <si>
-    <t>Muitos posts exploram a possibilidade de vida alienígena e tecnologia extraterrestre em relação ao 3I/ATLAS, com termos como 'nave Alien', 'OVNIs' e 'tecnología alien'. Há um forte fascínio pelo desconhecido no espaço, misturando ciência com teorias da conspiração e humor.</t>
-  </si>
-  <si>
-    <t>Disseminação de Notícias e Desinformação em Plataformas Digitais</t>
-  </si>
-  <si>
-    <t>O texto, sendo uma compilação de posts populares de uma plataforma como o TikTok, ilustra como informações (algumas verificadas, outras especulativas ou humorísticas) sobre eventos cósmicos e terrestres se espalham rapidamente, gerando milhões de visualizações e borrando a linha entre 'realidade e ficção', refletindo o fenômeno da viralização digital.</t>
-  </si>
-  <si>
-    <t>média</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -115,22 +60,81 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -418,78 +422,155 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="50" customWidth="1"/>
-    <col min="5" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col width="30" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="50" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="6"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Tema</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Descrição</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Relevância</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Roteiro</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Video Pronto</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Video Postado</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Data</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>O Objeto Interestelar 3I/ATLAS</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>O misterioso objeto 3I/ATLAS é o ponto central da maior parte do conteúdo, gerando intensas discussões sobre sua natureza – se é um cometa, um asteroide, um visitante de outra estrela ou até uma nave alienígena – e seu trajeto próximo ao Sol ou à Terra, com menções a datas específicas para revelações.</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>alta</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Roteiro TikTok: 3I/ATLAS – O Mistério Cósmico
+[Música de suspense crescente e vibrante, com uma batida forte e rápida de fundo]
+0-3 segundos: INTRODUÇÃO CHAMATIVA
+VISUAL: Começa com um close-up rápido e misterioso de um objeto cósmico brilhante se movendo no espaço, vindo do escuro. Flash de texto na tela: "O QUE É ISSO?" Corte rápido para uma simulação mais ampla de um objeto solitário no espaço, com um brilho incomum, simulando o 3I/ATLAS.
+VOZ: (Sussurro rápido e intenso, quase ofegante) "UM VISITANTE... DE OUTRA GALÁXIA?"
+TEXTO NA TELA: 👽 VISITA ALIENÍGENA? 🛸
+3-20 segundos: DESENVOLVIMENTO DO CONTEÚDO
+VISUAL: Sequência de cortes extremamente rápidos. Simulações do 3I/ATLAS se aproximando, gráficos simples e dinâmicos de trajetória espacial, cientistas em laboratório (imagens genéricas, rápidas), telescópios apontando para o céu.
+VOZ: (Tom animado, rápido e direto) "Você precisa conhecer o 3I/ATLAS! Esse objeto misterioso está deixando astrônomos de cabelo em pé no mundo todo!"
+TEXTO NA TELA: 🌌 O ENIGMA 3I/ATLAS!
+VOZ: "Não é um cometa comum, nem um asteroide qualquer. Ele veio de MUITO, MUITO LONGE! Tipo... de *fora* do nosso Sistema Solar! Isso mesmo, É INTERESTELAR!"
+TEXTO NA TELA: 🚀 ORIGEM INTERESTELAR!
+VISUAL: Ilustrações rápidas contrastando: um cometa tradicional (com cauda brilhante), um asteroide rochoso, e depois um objeto mais "limpo" ou com formato levemente incomum, com um brilho misterioso.
+VOZ: "A grande questão que todos se perguntam: é um cometa interestelar? Um asteroide super estranho? OU... *será que é algo mais*? Uma nave alienígena?"
+TEXTO NA TELA: COMETA? ASTEROIDE? 🛸 NAVE?
+VISUAL: Gráfico rápido e chamativo mostrando uma linha de trajetória passando *perto* do Sol e depois da órbita da Terra. Datas genéricas como "MÊS X" e "MÊS Y" piscam.
+VOZ: "Ele vai passar relativamente perto do Sol nos próximos meses, e teremos MAIS DADOS CRUCIAIS! Fique atento, as observações podem revelar tudo!"
+TEXTO NA TELA: 🔭 REVELAÇÕES A CAMINHO!
+20-30 segundos: CHAMADA PARA AÇÃO E CONCLUSÃO
+VISUAL: Imagem final do 3I/ATLAS flutuando no espaço profundo, com um grande ponto de interrogação cósmico piscando sobre ele. Música de suspense atinge o pico dramático e termina com um som de "ding" ou "whoosh" final e misterioso.
+VOZ: (Tom intrigante, mais lento e reflexivo) "E aí, qual sua teoria? Cometa exótico? Asteroide perdido? Ou estamos prestes a descobrir algo realmente extraordinário?"
+TEXTO NA TELA: 🤔 QUAL SUA TEORIA?
+VOZ: "Comenta AQUI embaixo o que você acha e me segue pra não perder NENHUMA atualização sobre o 3I/ATLAS! O universo... espera sua resposta!"
+TEXTO NA TELA: 👇 COMENTE! SIGA! 🔔
+[FADE OUT]</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Especulações sobre Vida Extraterrestre e Mistérios Cósmicos</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Muitos posts exploram a possibilidade de vida alienígena e tecnologia extraterrestre em relação ao 3I/ATLAS, com termos como 'nave Alien', 'OVNIs' e 'tecnología alien'. Há um forte fascínio pelo desconhecido no espaço, misturando ciência com teorias da conspiração e humor.</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>alta</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Disseminação de Notícias e Desinformação em Plataformas Digitais</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>O texto, sendo uma compilação de posts populares de uma plataforma como o TikTok, ilustra como informações (algumas verificadas, outras especulativas ou humorísticas) sobre eventos cósmicos e terrestres se espalham rapidamente, gerando milhões de visualizações e borrando a linha entre 'realidade e ficção', refletindo o fenômeno da viralização digital.</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>média</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Versão top de +
</commit_message>
<xml_diff>
--- a/planilha_temas.xlsx
+++ b/planilha_temas.xlsx
@@ -427,10 +427,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -636,6 +636,25 @@
           <t>alta</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>E se eu te dissesse que o caos no Rio de Janeiro já foi previsto, em detalhes, anos atrás? Preste atenção.
+Hoje, a cidade maravilhosa vive um pesadelo. Um clima de guerra. Megaoperações policiais se tornaram rotina, e a tensão nas ruas é quase palpável. Mas o que pouca gente sabe, é que esse cenário apocalíptico foi alertado. E não por qualquer um.
+Vídeos antigos, de lives no YouTube, ressurgiram, mostrando um profeta descrevendo exatamente o que vemos agora. Ele falava de uma 'megaoperação' que pararia o Rio, de um 'clima de guerra' que se instalaria na capital fluminense. De uma cidade em 'caos declarado'. Pense nos combates diários, nos desabafos desesperados de figuras públicas. Nas famílias vivendo sob fogo cruzado. Não é assustador como tudo se encaixa?
+Seria mera coincidência? Ou estamos testemunhando algo que transcende nossa compreensão, onde o sobrenatural se choca com a dura realidade social? Essa conexão é inegável, e aterrorizante.
+Agora me diz, você acredita nessa profecia? Deixe sua opinião e compartilhe esse vídeo. O mundo precisa saber disso.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -649,6 +668,163 @@
         </is>
       </c>
       <c r="C7" t="inlineStr">
+        <is>
+          <t>alta</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>O lendário 'gato fantasma' da Espanha? Ele é real e foi fotografado!
+Por séculos, histórias sussurravam sobre um felino espectral, uma sombra branca que vagava pelas montanhas da Península Ibérica. Ninguém nunca teve certeza… até agora. Em Jaén, na Espanha, um fotógrafo, numa noite que parecia como qualquer outra, registrou o impensável. Uma visão que parou o tempo e fez o mundo prender a respiração.
+Diante da câmera, ali estava ele: um lince-ibérico branco. Não albino, mas leucístico. Seus olhos, vibrantes e selvagens, contrastavam com a pelagem pura como a neve. Um lince! Uma espécie que mal sobreviveu ao fio da navalha da extinção, agora revela um exemplar tão único que reescreve a própria história. Você consegue imaginar a emoção desse momento? A beleza é chocante. Mas com essa raridade vem uma preocupação: essa pelagem, embora deslumbrante, compromete sua camuflagem natural. Um fantasma que, paradoxalmente, se tornou mais visível.
+Esse felino fantasma agora é real. E sua existência levanta uma pergunta assustadora: sua beleza será sua salvação ou sua perdição? Comente o que você pensa e compartilhe essa história inacreditável.</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-11-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Mistérios Cósmicos e Conspirações Alienígenas</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>O que a NASA realmente esconde sobre o Cometa 3I/ATLAS? Com mais de 200 milhões de visualizações em diversos vídeos, este 'cometa' é teorizado como uma nave alienígena por anomalias em sua trajetória, composição e comportamento ao se aproximar do Sol. A especulação sobre 'imagens secretas' do Telescópio James Webb e a insistência de cientistas renomados como Avi Loeb em sua natureza extraterrestre criam um suspense fascinante. Este tema alimenta a curiosidade, o medo do desconhecido e a busca por respostas sobre vida inteligente no universo, garantindo engajamento viral.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>alta</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Você sabia que o cometa mais misterioso da história pode não ser um cometa, mas sim… uma nave alienígena?
+Pouca gente sabe disso, mas o que vou te contar sobre o Cometa 3I/ATLAS é real... e pode mudar sua visão do universo. O ATLAS, com mais de 200 milhões de visualizações em vídeos, virou um enigma cósmico que a NASA insiste em chamar de rocha. Mas a verdade é que sua trajetória era estranha. Sua composição, mais ainda. Ao se aproximar do Sol, ele não se comportava como um cometa normal. Era como se estivesse... manobrando.
+Cientistas renomados, como Avi Loeb de Harvard, começaram a levantar a hipótese mais ousada: o ATLAS seria tecnologia extraterrestre. Uma nave disfarçada, observando a Terra. E o que a NASA realmente esconde? Há rumores insistentes de imagens secretas do Telescópio James Webb, que mostram algo além da nossa compreensão. Algo que foi rapidamente classificado, mas que levanta a pergunta: o que eles não querem que a gente veja?
+Enquanto o mundo dormia, os dados chegavam. As anomalias se acumulavam. Ninguém entendeu de fato o que estava acontecendo nos bastidores. Será que não estamos sozinhos? E se essa for a prova que sempre procuramos, escondida à vista de todos, por medo do que a revelação causaria?
+Isso muda tudo, não é? Agora me diz: você acredita que o Cometa ATLAS é uma nave alienígena? Comente sua teoria e mande esse vídeo pra quem precisa saber disso.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Heidi Klum e a Reinvenção do Halloween</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Ninguém domina o Halloween como Heidi Klum, cujos disfarces anuais são um fenômeno global que paralisam a internet. Cada ano, como em 2025 com sua Medusa hiper-realista e seu marido Tom Kaulitz transformado em pedra, seus trajes e a festa 'Heidiween' em Nova Iorque levam meses de planejamento e geram um misto de fascínio, choque e antecipação. A viralidade vem da transformação extrema, dos detalhes chocantes e da curiosidade em ver o que a 'rainha do Halloween' fará a seguir, provando que criatividade e espetáculo são receita para o sucesso.</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>alta</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Pouca gente entende a obsessão de Heidi Klum pelo Halloween. Mas o que eu vou te contar agora, vai mudar sua visão sobre a rainha do terror.
+Enquanto o mundo se prepara para uma noite de sustos e doces, Heidi já planeja há meses. A verdade é que ninguém, absolutamente NINGUÉM, domina o Halloween como ela. É um fenômeno global que paralisa a internet a cada ano, transformando Nova Iorque em seu palco sombrio.
+Você sabia que para 2025, os sussurros já apontam para uma Medusa hiper-realista, com escamas cintilantes e cobras que parecem rastejar? E seu marido, Tom Kaulitz, transformado em pedra, ao seu lado. É mais que uma fantasia; é uma obra de arte viva, uma cena de horror que ganha vida.
+Meses de trabalho, equipes de especialistas, detalhes tão chocantes que geram fascínio e repulsa. A 'Heidiween' não é só uma festa; é um ritual, uma antecipação do que a mente de Heidi Klum pode criar para nos chocar, nos intrigar. Você consegue imaginar o que é preciso para alcançar esse nível de transformação extrema?
+É essa mistura de criatividade insana e espetáculo puro que a torna a verdadeira rainha do Halloween. E cada ano, a pergunta ecoa: o que vem depois?
+Agora me diz... você teria coragem de encarar uma Medusa assim de perto? Manda esse vídeo pra quem precisa entender o verdadeiro poder de Heidi Klum.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Confrontos e Rivalidades de Personalidades</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>O Brasil parou para assistir a uma rivalidade explosiva que transcendeu as batalhas de rima e foi parar no ringue! A luta entre os MCs Xamuel e Jhony MC no Fight Music Show 7, que aconteceu em 01/11, gerou uma comoção nacional com milhões de visualizações em vídeos de prévias, encaradas tensas e reações pós-luta. A rivalidade acirrada, as provocações e a expectativa do confronto físico criaram um drama intenso e uma curiosidade imensa, alimentando debates sobre quem venceria e gerando conteúdos de reação em massa. Vídeos mostrando a encarada, falas polêmicas dos MCs e análises dos resultados são perfeitos para engajar a audiência com a tensão da disputa.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>alta</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Pouca gente sabe disso, mas uma rivalidade explosiva que parecia ficção parou o Brasil no dia 01 de novembro. O que começou em batalhas de rima, onde as palavras eram as armas, escalou para um nível que ninguém imaginava. Estamos falando de Xamuel e Jhony MC. Dois nomes que, por meses, trocaram farpas e promessas, alimentando uma tensão que era quase palpável nas redes sociais. Cada provocação, cada encarada tensa antes da luta... parecia um capítulo de um suspense. E então, no Fight Music Show 7, a contagem regressiva para o confronto físico chegou ao fim. As luzes do ringue focavam neles, enquanto milhões de olhos grudados nas telas esperavam o desfecho. O ar estava pesado, a expectativa era imensa. Quem venceria? Essa era a pergunta que ecoava em cada casa, em cada comentário. E o que aconteceu lá dentro do ringue? Bom, o resultado não só definiu um vencedor, mas reacendeu toda a chama dessa rivalidade, gerando uma onda de reações e análises que inundou a internet. Essa tensão parou um país inteiro. Mas e você, o que pensa sobre o papel da rivalidade nesses palcos? Será que é só espetáculo ou existe algo mais? Comente sua opinião e compartilhe essa história com seus amigos!</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-11-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Crises Urbanas e Segurança Pública</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Uma onda de medo e caos tomou conta do Rio de Janeiro, com operações policiais intensas que deixaram a população em alerta máximo! A recente megaoperação policial na cidade resultou em confrontos e gerou milhões de visualizações em vídeos de notícias, depoimentos de moradores e reações de personalidades como o ator André D'Lucca. A tensão das ruas, os relatos emocionantes de quem vive a realidade local, a presença policial e as discussões sobre violência e segurança pública criam um forte apelo emocional e um senso de urgência. Conteúdos que mostram a realidade da cidade, análises do impacto social e mensagens de solidariedade podem gerar grande engajamento e debate.</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>alta</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Transformações Impactantes de Celebridades</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Chocante! Heidi Klum, a rainha do Halloween, superou todas as expectativas com sua fantasia de Medusa, conquistando o título de melhor do mundo mais uma vez! Sua transformação inacreditável em Medusa para a tradicional festa 'Heidiween' em Nova York gerou mais de 558 milhões de visualizações, com detalhes impressionantes da maquiagem e do figurino. A curiosidade em torno da revelação, o impacto visual da criatividade e o suspense da transformação cativam o público, que busca ver o 'antes e depois' e os bastidores da criação. Vídeos que exploram o processo de elaboração da fantasia, a reação das pessoas e comparativos com anos anteriores geram fascínio e são altamente compartilháveis.</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>alta</t>
         </is>

</xml_diff>